<commit_message>
updated api for fecthing area
</commit_message>
<xml_diff>
--- a/LocationApi.xlsx
+++ b/LocationApi.xlsx
@@ -59,28 +59,10 @@
     <t>areas</t>
   </si>
   <si>
-    <t>/api/blocks/get/list/:districtCode/:stateCode/:countryCode</t>
-  </si>
-  <si>
-    <t>/api/districts/get/list/:stateCode/:countryCode</t>
-  </si>
-  <si>
-    <t>/api/states/get/list/:countryCode</t>
-  </si>
-  <si>
-    <t>/api/areas/get/list/:cityCode/:blockCode/:districtCode/:stateCode/:countryCode</t>
-  </si>
-  <si>
-    <t>/api/cities/get/list/:blockCode/:districtCode/:stateCode/:countryCode</t>
-  </si>
-  <si>
     <t>{ 
    area: String, 
    pincode: string
 }</t>
-  </si>
-  <si>
-    <t>/api/areas/get/one/:pincode</t>
   </si>
   <si>
     <t>{ 
@@ -98,15 +80,41 @@
   <si>
     <t>Done</t>
   </si>
+  <si>
+    <t>http://locationapi.iassureit.com/api/states/get/list/:countryCode</t>
+  </si>
+  <si>
+    <t>http://locationapi.iassureit.com/api/districts/get/list/:stateCode/:countryCode</t>
+  </si>
+  <si>
+    <t>http://locationapi.iassureit.com/api/areas/get/one/:pincode</t>
+  </si>
+  <si>
+    <t>http://locationapi.iassureit.com/api/blocks/get/list/:districtName/:stateCode/:countryCode</t>
+  </si>
+  <si>
+    <t>http://locationapi.iassureit.com/api/cities/get/list/:blockName/:districtName/:stateCode/:countryCode</t>
+  </si>
+  <si>
+    <t>http://locationapi.iassureit.com/api/areas/get/list/:cityName/:blockName/:districtName/:stateCode/:countryCode</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -135,10 +143,11 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
@@ -149,8 +158,12 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -432,7 +445,7 @@
   <dimension ref="A1:F14"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="D7" sqref="D7"/>
+      <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -462,7 +475,7 @@
         <v>5</v>
       </c>
       <c r="F1" s="2" t="s">
-        <v>19</v>
+        <v>13</v>
       </c>
     </row>
     <row r="2" spans="1:6" s="1" customFormat="1" ht="24" customHeight="1" x14ac:dyDescent="0.25">
@@ -472,11 +485,11 @@
       <c r="B2" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="C2" s="1" t="s">
-        <v>13</v>
+      <c r="C2" s="4" t="s">
+        <v>15</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>20</v>
+        <v>14</v>
       </c>
     </row>
     <row r="3" spans="1:6" s="1" customFormat="1" ht="24" customHeight="1" x14ac:dyDescent="0.25">
@@ -486,11 +499,11 @@
       <c r="B3" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="C3" s="1" t="s">
-        <v>12</v>
+      <c r="C3" s="4" t="s">
+        <v>16</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>20</v>
+        <v>14</v>
       </c>
     </row>
     <row r="4" spans="1:6" s="1" customFormat="1" ht="24" customHeight="1" x14ac:dyDescent="0.25">
@@ -500,11 +513,11 @@
       <c r="B4" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="C4" s="1" t="s">
-        <v>11</v>
+      <c r="C4" s="4" t="s">
+        <v>18</v>
       </c>
       <c r="F4" s="1" t="s">
-        <v>20</v>
+        <v>14</v>
       </c>
     </row>
     <row r="5" spans="1:6" s="1" customFormat="1" ht="24" customHeight="1" x14ac:dyDescent="0.25">
@@ -514,11 +527,11 @@
       <c r="B5" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="C5" s="1" t="s">
-        <v>15</v>
+      <c r="C5" s="4" t="s">
+        <v>19</v>
       </c>
       <c r="F5" s="1" t="s">
-        <v>20</v>
+        <v>14</v>
       </c>
     </row>
     <row r="6" spans="1:6" s="1" customFormat="1" ht="60" x14ac:dyDescent="0.25">
@@ -528,15 +541,15 @@
       <c r="B6" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="C6" s="1" t="s">
-        <v>14</v>
+      <c r="C6" s="4" t="s">
+        <v>20</v>
       </c>
       <c r="D6" s="3"/>
       <c r="E6" s="3" t="s">
-        <v>16</v>
+        <v>11</v>
       </c>
       <c r="F6" s="1" t="s">
-        <v>20</v>
+        <v>14</v>
       </c>
     </row>
     <row r="7" spans="1:6" s="1" customFormat="1" ht="85.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -546,14 +559,14 @@
       <c r="B7" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="C7" s="1" t="s">
+      <c r="C7" s="4" t="s">
         <v>17</v>
       </c>
       <c r="E7" s="3" t="s">
-        <v>18</v>
+        <v>12</v>
       </c>
       <c r="F7" s="1" t="s">
-        <v>20</v>
+        <v>14</v>
       </c>
     </row>
     <row r="8" spans="1:6" s="1" customFormat="1" ht="24" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -564,6 +577,14 @@
     <row r="13" spans="1:6" s="1" customFormat="1" ht="24" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="14" spans="1:6" s="1" customFormat="1" ht="24" customHeight="1" x14ac:dyDescent="0.25"/>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="C2" r:id="rId1"/>
+    <hyperlink ref="C3" r:id="rId2"/>
+    <hyperlink ref="C4" r:id="rId3"/>
+    <hyperlink ref="C5" r:id="rId4"/>
+    <hyperlink ref="C6" r:id="rId5"/>
+    <hyperlink ref="C7" r:id="rId6"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Priyanka kale added subarea, society related changes
</commit_message>
<xml_diff>
--- a/LocationApi.xlsx
+++ b/LocationApi.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="41">
   <si>
     <t>Collection</t>
   </si>
@@ -57,12 +57,6 @@
   </si>
   <si>
     <t>areas</t>
-  </si>
-  <si>
-    <t>{ 
-   area: String, 
-   pincode: string
-}</t>
   </si>
   <si>
     <t>{ 
@@ -97,6 +91,94 @@
   </si>
   <si>
     <t>http://locationapi.iassureit.com/api/areas/get/list/:cityName/:blockName/:districtName/:stateCode/:countryCode</t>
+  </si>
+  <si>
+    <t xml:space="preserve">API </t>
+  </si>
+  <si>
+    <t>States</t>
+  </si>
+  <si>
+    <t>Districts</t>
+  </si>
+  <si>
+    <t>Blocks</t>
+  </si>
+  <si>
+    <t>BlocksByState</t>
+  </si>
+  <si>
+    <t>http://locationapi.iassureit.com/api/blocks/get/BlocksByState/:stateCode/:countryCode</t>
+  </si>
+  <si>
+    <t>Villages</t>
+  </si>
+  <si>
+    <t>Areas</t>
+  </si>
+  <si>
+    <t>Details By Pincoe</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Search location </t>
+  </si>
+  <si>
+    <t>http://locationapi.iassureit.com/api/areas/get/list/searchByAreaBlock/Str</t>
+  </si>
+  <si>
+    <t>http://locationapi.iassureit.com/api/areas/get/areaDetails/Hadapsar S.O</t>
+  </si>
+  <si>
+    <t>areaDetails</t>
+  </si>
+  <si>
+    <t>insertSubArea</t>
+  </si>
+  <si>
+    <t>post</t>
+  </si>
+  <si>
+    <t>/api/subareas/post</t>
+  </si>
+  <si>
+    <t>{
+ "countryCode"    : "IN",
+    "stateName"      : "MH",
+    "districtName"   : "Pune",
+    "blockName"      : "Bhor",
+    "areaName"       : "Hadapsar S.O",
+    "subareaName"    : "Hadapsar"
+  }</t>
+  </si>
+  <si>
+    <t>done</t>
+  </si>
+  <si>
+    <t>subarea</t>
+  </si>
+  <si>
+    <t>[{
+        "_id": "5d4a5ff4fc34542228e3f7fb",
+        "countryCode": "IN",
+        "stateName": "Maharashtra",
+        "stateCode": "MH",
+        "districtName": "amravati",
+        "blockName": "achalpur",
+        "pincode": ""
+    }]</t>
+  </si>
+  <si>
+    <t>[
+    {
+        "_id": "5d4153a7dd5de32438d6f61e",
+        "countryCode": "IN",
+        "stateName": "MAHARASHTRA",
+        "stateCode": "MH",
+        "districtName": "Pune",
+        "blockName": "Pune City",
+        "areaName": "9 DRD B.O",
+        "pincode": "411014"
+    }]</t>
   </si>
 </sst>
 </file>
@@ -147,7 +229,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
@@ -160,6 +242,10 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyAlignment="1">
       <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -442,149 +528,236 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F14"/>
+  <dimension ref="A1:G15"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+    <sheetView tabSelected="1" topLeftCell="D6" workbookViewId="0">
+      <selection activeCell="G7" sqref="G7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="20.140625" customWidth="1"/>
-    <col min="2" max="2" width="20" customWidth="1"/>
-    <col min="3" max="3" width="78.28515625" customWidth="1"/>
-    <col min="4" max="4" width="26.7109375" customWidth="1"/>
-    <col min="5" max="5" width="33.5703125" customWidth="1"/>
-    <col min="6" max="6" width="27.28515625" customWidth="1"/>
+    <col min="2" max="3" width="20" customWidth="1"/>
+    <col min="4" max="4" width="78.28515625" customWidth="1"/>
+    <col min="5" max="5" width="26.7109375" customWidth="1"/>
+    <col min="6" max="6" width="33.5703125" customWidth="1"/>
+    <col min="7" max="7" width="27.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="C1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="D1" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="E1" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="F1" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="F1" s="2" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6" s="1" customFormat="1" ht="24" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="G1" s="2" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" s="1" customFormat="1" ht="24" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>6</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="C2" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="F2" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D2" s="4" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="3" spans="1:6" s="1" customFormat="1" ht="24" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="G2" s="1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" s="1" customFormat="1" ht="24" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>7</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="C3" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="F3" s="1" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" s="1" customFormat="1" ht="24" customHeight="1" x14ac:dyDescent="0.25">
+        <v>22</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D3" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="G3" s="1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" s="1" customFormat="1" ht="24" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>8</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="C4" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D4" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="G4" s="1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" ht="150" x14ac:dyDescent="0.25">
+      <c r="B5" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D5" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="F5" s="6" t="s">
+        <v>39</v>
+      </c>
+      <c r="G5" s="1" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" s="1" customFormat="1" ht="24" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D6" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="F4" s="1" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" s="1" customFormat="1" ht="24" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="B5" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="C5" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="F5" s="1" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" s="1" customFormat="1" ht="60" x14ac:dyDescent="0.25">
-      <c r="A6" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="B6" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="C6" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="D6" s="3"/>
-      <c r="E6" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="F6" s="1" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6" s="1" customFormat="1" ht="85.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="G6" s="1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" s="1" customFormat="1" ht="180" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>10</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="C7" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="E7" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="F7" s="1" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6" s="1" customFormat="1" ht="24" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="9" spans="1:6" s="1" customFormat="1" ht="24" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="10" spans="1:6" s="1" customFormat="1" ht="24" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="11" spans="1:6" s="1" customFormat="1" ht="24" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="12" spans="1:6" s="1" customFormat="1" ht="24" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="13" spans="1:6" s="1" customFormat="1" ht="24" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="14" spans="1:6" s="1" customFormat="1" ht="24" customHeight="1" x14ac:dyDescent="0.25"/>
+        <v>27</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D7" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="E7" s="3"/>
+      <c r="F7" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="G7" s="1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" s="1" customFormat="1" ht="85.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D8" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="F8" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="G8" s="1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" s="1" customFormat="1" ht="24" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D9" s="4" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" s="1" customFormat="1" ht="24" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D10" s="5" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" s="1" customFormat="1" ht="126" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="C11" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="D11" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="F11" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="G11" s="1" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" s="1" customFormat="1" ht="24" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="13" spans="1:7" s="1" customFormat="1" ht="24" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="14" spans="1:7" s="1" customFormat="1" ht="24" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="15" spans="1:7" s="1" customFormat="1" ht="24" customHeight="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="C2" r:id="rId1"/>
-    <hyperlink ref="C3" r:id="rId2"/>
-    <hyperlink ref="C4" r:id="rId3"/>
-    <hyperlink ref="C5" r:id="rId4"/>
-    <hyperlink ref="C6" r:id="rId5"/>
-    <hyperlink ref="C7" r:id="rId6"/>
+    <hyperlink ref="D2" r:id="rId1"/>
+    <hyperlink ref="D3" r:id="rId2"/>
+    <hyperlink ref="D4" r:id="rId3"/>
+    <hyperlink ref="D6" r:id="rId4"/>
+    <hyperlink ref="D7" r:id="rId5"/>
+    <hyperlink ref="D8" r:id="rId6"/>
+    <hyperlink ref="D5" r:id="rId7"/>
+    <hyperlink ref="D9" r:id="rId8"/>
+    <hyperlink ref="D10" r:id="rId9"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId10"/>
 </worksheet>
 </file>
</xml_diff>